<commit_message>
° symbol in readData
</commit_message>
<xml_diff>
--- a/dataUncert/testData/data6.xlsx
+++ b/dataUncert/testData/data6.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ymerdkdc01\folder redirections\DJAVE\My Documents\GitHub\dataUncert\dataUncert\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24FCAE6-36BD-4126-8256-DA2B9403955F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4736CBB-773D-48F4-99EE-0065AA59BCE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F5F6BAB0-B9A3-4FB8-B84A-62DE77F5D537}"/>
   </bookViews>
@@ -40,13 +40,13 @@
     <t>A</t>
   </si>
   <si>
-    <t>L/min</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
     <t>mA</t>
+  </si>
+  <si>
+    <t>°</t>
   </si>
 </sst>
 </file>
@@ -401,20 +401,20 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -422,16 +422,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
       <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>